<commit_message>
RTM without tags test cases
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Doc/SRS_4.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Doc/SRS_4.xlsx
@@ -171,10 +171,6 @@
     <t>SR6_A01</t>
   </si>
   <si>
-    <t xml:space="preserve">this function inside the application,user will choose between Speed Range ,it's configurable as user want   .
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">this function inside application, there is four switches in the system                                                           1- Selection Button
    2-Increase Button
                                                                        3-Decrease Button                                                                   4-On/Off Button 
@@ -192,6 +188,10 @@
   </si>
   <si>
     <t xml:space="preserve">switches of system will be Tactile (optional)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this function inside the application,user will choose between Speed Range ,it's configurable as user want by calling u8 ChangeSpeed(u8 Speed) this function take one argument and return Error/ok dependant on the speed that user choose  .
 </t>
   </si>
 </sst>
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -920,12 +920,12 @@
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C18" s="8"/>
     </row>
@@ -934,25 +934,25 @@
         <v>43</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="C21" s="8"/>
     </row>

</xml_diff>